<commit_message>
ajout MCD + update journal de travail
</commit_message>
<xml_diff>
--- a/C#_JournalDeTravail_KGS_MMO_SGI.xlsx
+++ b/C#_JournalDeTravail_KGS_MMO_SGI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MA\Projet C#\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MA\Projet C#\github_c#\Projet-C_KGS_MMO_SGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nom</t>
   </si>
@@ -62,10 +62,19 @@
     <t>1h30</t>
   </si>
   <si>
-    <t>Organisation base de données, et création MCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fin de création de MCD, </t>
+    <t>planification de la base de données, et création MCD</t>
+  </si>
+  <si>
+    <t>3h45</t>
+  </si>
+  <si>
+    <t>création de git, ajout des stories dans icescrum et fin de la création de MCD. Création du MLD</t>
+  </si>
+  <si>
+    <t>On s'est planifié sur quels types de tables il y aurait, et on a également commencé a effectuer le MCD</t>
+  </si>
+  <si>
+    <t>Meeting avec le professeur, nous avons crée un dépôt git et ajouté des stories dans icescrum. Le MCD est terminé. Nous avons commencé a créer le MLD</t>
   </si>
 </sst>
 </file>
@@ -436,7 +445,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>44518</v>
       </c>
@@ -508,9 +517,11 @@
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>44523</v>
       </c>
@@ -518,164 +529,168 @@
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="5"/>
       <c r="C20" s="8"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>

</xml_diff>